<commit_message>
update inbound record and summary export
更新订单号至汇总excel导出
</commit_message>
<xml_diff>
--- a/backend-python/general_document/财务入库总单模板.xlsx
+++ b/backend-python/general_document/财务入库总单模板.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>财务部入库总单</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>入库单据号</t>
+  </si>
+  <si>
+    <t>订单号</t>
   </si>
   <si>
     <t>入库时间</t>
@@ -720,7 +723,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -730,16 +733,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1061,149 +1055,158 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="27.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="1"/>
-    <col min="10" max="10" width="11.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="2" max="2" width="17.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9" style="1"/>
+    <col min="11" max="11" width="11.125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="31.5" spans="1:11">
+    <row r="1" ht="31.5" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="4" t="s">
+    <row r="2" ht="18.75" spans="1:12">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
-    <row r="3" ht="9" customHeight="1" spans="1:11">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+    <row r="3" ht="9" customHeight="1" spans="1:12">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
     </row>
-    <row r="4" ht="6" customHeight="1" spans="1:11">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
+    <row r="4" ht="6" customHeight="1" spans="1:12">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+    <row r="5" spans="1:12">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:12">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="E2:E4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="F2:G4"/>
-    <mergeCell ref="I2:K4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="B2:C4"/>
+    <mergeCell ref="G2:H4"/>
+    <mergeCell ref="J2:L4"/>
   </mergeCells>
   <pageMargins left="0.196527777777778" right="0.196527777777778" top="0.196527777777778" bottom="0.196527777777778" header="0.196527777777778" footer="0.196527777777778"/>
   <pageSetup paperSize="9" scale="94" fitToHeight="0" orientation="landscape" horizontalDpi="600"/>

</xml_diff>